<commit_message>
Rename STATA data columns
</commit_message>
<xml_diff>
--- a/stata_data.xlsx
+++ b/stata_data.xlsx
@@ -476,22 +476,22 @@
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>% Change in Growth Rate (t=1)</t>
+          <t>one_m_diff</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>% Change in Growth Rate (t=3)</t>
+          <t>three_m_diff</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>% Change in Growth Rate (t=6)</t>
+          <t>six_m_diff</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>% Change in Growth Rate (t=12)</t>
+          <t>one_y_diff</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Ran Summary Stats and OLS on New Design Matrix
</commit_message>
<xml_diff>
--- a/stata_data.xlsx
+++ b/stata_data.xlsx
@@ -482,42 +482,42 @@
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>% Change in Volume (t=1)</t>
+          <t>one_m_diff_volume</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>% Change in Volume (t=3)</t>
+          <t>three_m_diff_volume</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
         <is>
-          <t>% Change in Volume (t=6)</t>
+          <t>six_m_diff_volume</t>
         </is>
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>% Change in Volume (t=12)</t>
+          <t>one_y_diff_volume</t>
         </is>
       </c>
       <c r="J1" s="1" t="inlineStr">
         <is>
-          <t>% Change in Share Price (t=1)</t>
+          <t>one_m_diff_shareprice</t>
         </is>
       </c>
       <c r="K1" s="1" t="inlineStr">
         <is>
-          <t>% Change in Share Price (t=3)</t>
+          <t>three_m_diff_shareprice</t>
         </is>
       </c>
       <c r="L1" s="1" t="inlineStr">
         <is>
-          <t>% Change in Share Price (t=6)</t>
+          <t>six_m_diff_shareprice</t>
         </is>
       </c>
       <c r="M1" s="1" t="inlineStr">
         <is>
-          <t>% Change in Share Price (t=12)</t>
+          <t>one_y_diff_shareprice</t>
         </is>
       </c>
     </row>

</xml_diff>